<commit_message>
Refactor Express setup and update state diagram
Cleaned up Express app initialization in index.ts by removing commented and redundant code. Fixed import and route registration for funcionarios in routes/index.ts. Updated state diagram descriptions in DEstados.plantuml and regenerated the corresponding PNG. Updated internal schedule spreadsheet.
</commit_message>
<xml_diff>
--- a/Documentos Internos/Cronograma.xlsx
+++ b/Documentos Internos/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\22996_22997_23008_23015_23020\Documentos Internos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\GitHub\PDM_PA_50_10\Documentos Internos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEDD725-E6F6-410E-9E8D-EB2101CFF25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B09AF3-809F-4592-8BB6-87F8088D459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -278,9 +278,6 @@
     <t>:: Diagrama de modelo de dados (ER) </t>
   </si>
   <si>
-    <t>::Diagrama de dominio</t>
-  </si>
-  <si>
     <t>::Diagrama de Estados</t>
   </si>
   <si>
@@ -639,6 +636,9 @@
   </si>
   <si>
     <t>Data Final</t>
+  </si>
+  <si>
+    <t>:: Diagrama de dominio</t>
   </si>
 </sst>
 </file>
@@ -953,17 +953,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1276,37 +1276,37 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="25" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="25" t="s">
+      <c r="J1" s="31"/>
+      <c r="K1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="25" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="25" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="26"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="30">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
@@ -1342,7 +1342,7 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="60">
-      <c r="A3" s="28"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>26</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O3" s="3">
         <v>27</v>
@@ -1380,7 +1380,7 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" ht="44.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="82.5" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2">
@@ -1451,7 +1451,7 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="45">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2">
         <v>7</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="3">
         <v>14</v>
@@ -1486,7 +1486,7 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" ht="44.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2">
         <v>9</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="45">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2">
@@ -1572,7 +1572,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="3">
         <v>4</v>
@@ -1596,7 +1596,7 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2">
         <v>11</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2">
         <v>12</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" ht="45">
-      <c r="A12" s="28"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2">
         <v>13</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="3">
         <v>25</v>
@@ -1700,7 +1700,7 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" ht="60">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
@@ -1731,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O13" s="3">
         <v>6</v>
@@ -1739,7 +1739,7 @@
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2">
         <v>15</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" ht="45">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2">
         <v>16</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G15" s="3">
         <v>16</v>
@@ -1809,7 +1809,7 @@
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2">
         <v>17</v>
       </c>
@@ -1843,7 +1843,7 @@
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2">
         <v>18</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="28" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2">
@@ -1915,7 +1915,7 @@
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" ht="30">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -1946,11 +1946,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
@@ -1958,6 +1953,11 @@
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{0A4A7E6F-5B19-4043-8AA1-14A479757A24}"/>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895AAF2E-62E0-4D99-9699-CE3C7B3F175D}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2061,54 +2061,54 @@
       <c r="B14" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" ht="15.75">
       <c r="A15" s="17"/>
       <c r="B15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:5" ht="15.75">
       <c r="A16" s="17"/>
       <c r="B16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="17"/>
       <c r="B17" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="17"/>
       <c r="B18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="19"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" ht="15.75">
       <c r="A21" s="22" t="s">
@@ -2130,13 +2130,13 @@
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75">
+      <c r="A25" s="24" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" s="17"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75">
-      <c r="A25" s="20" t="s">
-        <v>47</v>
       </c>
       <c r="B25" s="17"/>
     </row>
@@ -2161,7 +2161,7 @@
     <row r="29" spans="1:5" ht="15.75">
       <c r="A29" s="17"/>
       <c r="B29" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75">
@@ -2170,25 +2170,25 @@
     </row>
     <row r="31" spans="1:5" ht="15.75">
       <c r="A31" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="22"/>
     </row>
     <row r="32" spans="1:5" ht="15.75">
       <c r="A32" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="22"/>
     </row>
     <row r="33" spans="1:2" ht="15.75">
       <c r="A33" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33" s="17"/>
     </row>
     <row r="34" spans="1:2" ht="15.75">
       <c r="A34" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="17"/>
     </row>
@@ -2201,12 +2201,12 @@
     <row r="36" spans="1:2" ht="15.75">
       <c r="A36" s="17"/>
       <c r="B36" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75">
       <c r="A37" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="17"/>
     </row>
@@ -2216,13 +2216,13 @@
     </row>
     <row r="39" spans="1:2" ht="15.75">
       <c r="A39" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="22"/>
     </row>
     <row r="40" spans="1:2" ht="15.75">
       <c r="A40" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="22"/>
     </row>
@@ -2234,19 +2234,19 @@
     </row>
     <row r="42" spans="1:2" ht="15.75">
       <c r="A42" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="17"/>
     </row>
     <row r="43" spans="1:2" ht="15.75">
       <c r="A43" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="17"/>
     </row>
     <row r="44" spans="1:2" ht="15.75">
       <c r="A44" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" s="17"/>
     </row>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="47" spans="1:2" ht="15.75">
       <c r="A47" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" s="17"/>
     </row>
@@ -2272,19 +2272,19 @@
     </row>
     <row r="49" spans="1:2" ht="15.75">
       <c r="A49" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="17"/>
     </row>
     <row r="50" spans="1:2" ht="15.75">
       <c r="A50" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="17"/>
     </row>
     <row r="51" spans="1:2" ht="15.75">
       <c r="A51" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" s="17"/>
     </row>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="53" spans="1:2" ht="15.75">
       <c r="A53" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B53" s="17"/>
     </row>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="55" spans="1:2" ht="15.75">
       <c r="A55" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="17"/>
     </row>
     <row r="56" spans="1:2" ht="15.75">
       <c r="A56" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56" s="17"/>
     </row>
@@ -2343,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866E5C1-172E-4782-AFD1-E9BEE95982AD}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -2359,1463 +2359,1463 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="D1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="K1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="L1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="M1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="N1" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="O1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="P1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="Q1" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="30" t="s">
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="26" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="30" t="s">
+      <c r="B2" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="C2" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="D2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="E2" s="27">
+        <v>45950.510974328703</v>
+      </c>
+      <c r="F2" s="27">
+        <v>45950.511443263887</v>
+      </c>
+      <c r="G2" s="27">
+        <v>45950.511442997682</v>
+      </c>
+      <c r="H2" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="31">
-        <v>45950.510974328703</v>
-      </c>
-      <c r="F2" s="31">
-        <v>45950.511443263887</v>
-      </c>
-      <c r="G2" s="31">
-        <v>45950.511442997682</v>
-      </c>
-      <c r="H2" s="30" t="s">
+      <c r="I2" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="J2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="K2" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="L2" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="M2" s="26">
+        <v>0</v>
+      </c>
+      <c r="N2" s="26">
+        <v>0</v>
+      </c>
+      <c r="O2" s="26">
+        <v>0</v>
+      </c>
+      <c r="P2" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="30">
-        <v>0</v>
-      </c>
-      <c r="N2" s="30">
-        <v>0</v>
-      </c>
-      <c r="O2" s="30">
-        <v>0</v>
-      </c>
-      <c r="P2" s="30" t="s">
+      <c r="Q2" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="Q2" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="30" t="s">
+      <c r="B3" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="E3" s="27">
+        <v>45950.511326782405</v>
+      </c>
+      <c r="F3" s="27">
+        <v>45950.511428182872</v>
+      </c>
+      <c r="G3" s="27">
+        <v>45950.511427962963</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="26">
+        <v>0</v>
+      </c>
+      <c r="N3" s="26">
+        <v>0</v>
+      </c>
+      <c r="O3" s="26">
+        <v>0</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="31">
-        <v>45950.511326782405</v>
-      </c>
-      <c r="F3" s="31">
-        <v>45950.511428182872</v>
-      </c>
-      <c r="G3" s="31">
-        <v>45950.511427962963</v>
-      </c>
-      <c r="H3" s="30" t="s">
+      <c r="D4" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="27">
+        <v>45943.456266875</v>
+      </c>
+      <c r="F4" s="27">
+        <v>45950.51083324074</v>
+      </c>
+      <c r="G4" s="27">
+        <v>45950.510832662039</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="J4" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" s="30" t="s">
+      <c r="K4" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="26">
+        <v>0</v>
+      </c>
+      <c r="N4" s="26">
+        <v>0</v>
+      </c>
+      <c r="O4" s="26">
+        <v>0</v>
+      </c>
+      <c r="P4" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="30">
-        <v>0</v>
-      </c>
-      <c r="N3" s="30">
-        <v>0</v>
-      </c>
-      <c r="O3" s="30">
-        <v>0</v>
-      </c>
-      <c r="P3" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q3" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="30" t="s">
+      <c r="Q4" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="30" t="s">
+      <c r="D5" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="27">
+        <v>45943.430894224533</v>
+      </c>
+      <c r="F5" s="27">
+        <v>45950.510795879629</v>
+      </c>
+      <c r="G5" s="27">
+        <v>45950.510795578703</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="31">
-        <v>45943.456266875</v>
-      </c>
-      <c r="F4" s="31">
-        <v>45950.51083324074</v>
-      </c>
-      <c r="G4" s="31">
-        <v>45950.510832662039</v>
-      </c>
-      <c r="H4" s="30" t="s">
+      <c r="L5" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="26">
+        <v>0</v>
+      </c>
+      <c r="N5" s="26">
+        <v>0</v>
+      </c>
+      <c r="O5" s="26">
+        <v>0</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="27">
+        <v>45943.430709548615</v>
+      </c>
+      <c r="F6" s="27">
+        <v>45950.510774305556</v>
+      </c>
+      <c r="G6" s="27">
+        <v>45950.510773969909</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="J6" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="J4" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K4" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="L4" s="30" t="s">
+      <c r="K6" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="26">
+        <v>0</v>
+      </c>
+      <c r="N6" s="26">
+        <v>3</v>
+      </c>
+      <c r="O6" s="26">
+        <v>0</v>
+      </c>
+      <c r="P6" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M4" s="30">
-        <v>0</v>
-      </c>
-      <c r="N4" s="30">
-        <v>0</v>
-      </c>
-      <c r="O4" s="30">
-        <v>0</v>
-      </c>
-      <c r="P4" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q4" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="30" t="s">
+      <c r="Q6" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="30" t="s">
+      <c r="D7" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="27">
+        <v>45943.430474560184</v>
+      </c>
+      <c r="F7" s="27">
+        <v>45950.510754479168</v>
+      </c>
+      <c r="G7" s="27">
+        <v>45950.510754120369</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M7" s="26">
+        <v>0</v>
+      </c>
+      <c r="N7" s="26">
+        <v>0</v>
+      </c>
+      <c r="O7" s="26">
+        <v>0</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="27">
+        <v>45940.606958912038</v>
+      </c>
+      <c r="F8" s="27">
+        <v>45950.510734664349</v>
+      </c>
+      <c r="G8" s="27">
+        <v>45950.510734444448</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="26">
+        <v>0</v>
+      </c>
+      <c r="N8" s="26">
+        <v>0</v>
+      </c>
+      <c r="O8" s="26">
+        <v>0</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="27">
+        <v>45943.431502662039</v>
+      </c>
+      <c r="F9" s="27">
+        <v>45950.510677638886</v>
+      </c>
+      <c r="G9" s="27">
+        <v>45950.510677256942</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="26">
+        <v>0</v>
+      </c>
+      <c r="N9" s="26">
+        <v>0</v>
+      </c>
+      <c r="O9" s="26">
+        <v>0</v>
+      </c>
+      <c r="P9" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="27">
+        <v>45943.45384840278</v>
+      </c>
+      <c r="F10" s="27">
+        <v>45950.519420578705</v>
+      </c>
+      <c r="G10" s="27"/>
+      <c r="H10" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="M10" s="26">
+        <v>0</v>
+      </c>
+      <c r="N10" s="26">
+        <v>0</v>
+      </c>
+      <c r="O10" s="26">
+        <v>0</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="27">
+        <v>45940.607197754631</v>
+      </c>
+      <c r="F11" s="27">
+        <v>45950.519361666666</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K11" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="31">
-        <v>45943.430894224533</v>
-      </c>
-      <c r="F5" s="31">
-        <v>45950.510795879629</v>
-      </c>
-      <c r="G5" s="31">
-        <v>45950.510795578703</v>
-      </c>
-      <c r="H5" s="30" t="s">
+      <c r="L11" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" s="26">
+        <v>0</v>
+      </c>
+      <c r="N11" s="26">
+        <v>0</v>
+      </c>
+      <c r="O11" s="26">
+        <v>0</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="27">
+        <v>45947.650316388892</v>
+      </c>
+      <c r="F12" s="27">
+        <v>45950.519264664355</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="L5" s="30" t="s">
+      <c r="J12" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="M12" s="26">
+        <v>0</v>
+      </c>
+      <c r="N12" s="26">
+        <v>0</v>
+      </c>
+      <c r="O12" s="26">
+        <v>0</v>
+      </c>
+      <c r="P12" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M5" s="30">
-        <v>0</v>
-      </c>
-      <c r="N5" s="30">
-        <v>0</v>
-      </c>
-      <c r="O5" s="30">
-        <v>0</v>
-      </c>
-      <c r="P5" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q5" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="30" t="s">
+      <c r="Q12" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="31">
-        <v>45943.430709548615</v>
-      </c>
-      <c r="F6" s="31">
-        <v>45950.510774305556</v>
-      </c>
-      <c r="G6" s="31">
-        <v>45950.510773969909</v>
-      </c>
-      <c r="H6" s="30" t="s">
+      <c r="D13" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="27">
+        <v>45943.454216377315</v>
+      </c>
+      <c r="F13" s="27">
+        <v>45950.519221319446</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" s="30" t="s">
+      <c r="J13" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" s="26">
+        <v>0</v>
+      </c>
+      <c r="N13" s="26">
+        <v>0</v>
+      </c>
+      <c r="O13" s="26">
+        <v>0</v>
+      </c>
+      <c r="P13" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M6" s="30">
-        <v>0</v>
-      </c>
-      <c r="N6" s="30">
-        <v>3</v>
-      </c>
-      <c r="O6" s="30">
-        <v>0</v>
-      </c>
-      <c r="P6" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q6" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="30" t="s">
+      <c r="Q13" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="31">
-        <v>45943.430474560184</v>
-      </c>
-      <c r="F7" s="31">
-        <v>45950.510754479168</v>
-      </c>
-      <c r="G7" s="31">
-        <v>45950.510754120369</v>
-      </c>
-      <c r="H7" s="30" t="s">
+      <c r="D14" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="27">
+        <v>45950.457830729167</v>
+      </c>
+      <c r="F14" s="27">
+        <v>45950.513444525466</v>
+      </c>
+      <c r="G14" s="27"/>
+      <c r="H14" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I7" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="L7" s="30" t="s">
+      <c r="J14" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="M14" s="26">
+        <v>0</v>
+      </c>
+      <c r="N14" s="26">
+        <v>0</v>
+      </c>
+      <c r="O14" s="26">
+        <v>0</v>
+      </c>
+      <c r="P14" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M7" s="30">
-        <v>0</v>
-      </c>
-      <c r="N7" s="30">
-        <v>0</v>
-      </c>
-      <c r="O7" s="30">
-        <v>0</v>
-      </c>
-      <c r="P7" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q7" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="30" t="s">
+      <c r="Q14" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="31">
-        <v>45940.606958912038</v>
-      </c>
-      <c r="F8" s="31">
-        <v>45950.510734664349</v>
-      </c>
-      <c r="G8" s="31">
-        <v>45950.510734444448</v>
-      </c>
-      <c r="H8" s="30" t="s">
+      <c r="D15" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="27">
+        <v>45950.45394861111</v>
+      </c>
+      <c r="F15" s="27">
+        <v>45950.513370104163</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="L8" s="30" t="s">
+      <c r="J15" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="M15" s="26">
+        <v>0</v>
+      </c>
+      <c r="N15" s="26">
+        <v>0</v>
+      </c>
+      <c r="O15" s="26">
+        <v>0</v>
+      </c>
+      <c r="P15" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M8" s="30">
-        <v>0</v>
-      </c>
-      <c r="N8" s="30">
-        <v>0</v>
-      </c>
-      <c r="O8" s="30">
-        <v>0</v>
-      </c>
-      <c r="P8" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q8" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="30" t="s">
+      <c r="Q15" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" s="31">
-        <v>45943.431502662039</v>
-      </c>
-      <c r="F9" s="31">
-        <v>45950.510677638886</v>
-      </c>
-      <c r="G9" s="31">
-        <v>45950.510677256942</v>
-      </c>
-      <c r="H9" s="30" t="s">
+      <c r="D16" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="27">
+        <v>45950.512167835652</v>
+      </c>
+      <c r="F16" s="27">
+        <v>45950.51362597222</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="L9" s="30" t="s">
+      <c r="J16" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="M16" s="26">
+        <v>0</v>
+      </c>
+      <c r="N16" s="26">
+        <v>0</v>
+      </c>
+      <c r="O16" s="26">
+        <v>0</v>
+      </c>
+      <c r="P16" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="M9" s="30">
-        <v>0</v>
-      </c>
-      <c r="N9" s="30">
-        <v>0</v>
-      </c>
-      <c r="O9" s="30">
-        <v>0</v>
-      </c>
-      <c r="P9" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q9" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="30" t="s">
+      <c r="Q16" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="30" t="s">
+      <c r="D17" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="27">
+        <v>45950.512106817128</v>
+      </c>
+      <c r="F17" s="27">
+        <v>45950.513540092594</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="31">
-        <v>45943.45384840278</v>
-      </c>
-      <c r="F10" s="31">
-        <v>45950.519420578705</v>
-      </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="30" t="s">
+      <c r="K17" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L17" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="M17" s="26">
+        <v>0</v>
+      </c>
+      <c r="N17" s="26">
+        <v>0</v>
+      </c>
+      <c r="O17" s="26">
+        <v>0</v>
+      </c>
+      <c r="P17" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" s="27">
+        <v>45950.506588495373</v>
+      </c>
+      <c r="F18" s="27">
+        <v>45950.506588495373</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="L10" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="M10" s="30">
-        <v>0</v>
-      </c>
-      <c r="N10" s="30">
-        <v>0</v>
-      </c>
-      <c r="O10" s="30">
-        <v>0</v>
-      </c>
-      <c r="P10" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q10" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="30" t="s">
+      <c r="J18" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="M18" s="26">
+        <v>0</v>
+      </c>
+      <c r="N18" s="26">
+        <v>0</v>
+      </c>
+      <c r="O18" s="26">
+        <v>0</v>
+      </c>
+      <c r="P18" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="31">
-        <v>45940.607197754631</v>
-      </c>
-      <c r="F11" s="31">
-        <v>45950.519361666666</v>
-      </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30" t="s">
+      <c r="D19" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="27">
+        <v>45950.506292314814</v>
+      </c>
+      <c r="F19" s="27">
+        <v>45950.506292314814</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="L11" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="M11" s="30">
-        <v>0</v>
-      </c>
-      <c r="N11" s="30">
-        <v>0</v>
-      </c>
-      <c r="O11" s="30">
-        <v>0</v>
-      </c>
-      <c r="P11" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q11" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="30" t="s">
+      <c r="J19" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="26">
+        <v>0</v>
+      </c>
+      <c r="N19" s="26">
+        <v>0</v>
+      </c>
+      <c r="O19" s="26">
+        <v>0</v>
+      </c>
+      <c r="P19" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q19" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="31">
-        <v>45947.650316388892</v>
-      </c>
-      <c r="F12" s="31">
-        <v>45950.519264664355</v>
-      </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="30" t="s">
+      <c r="D20" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="27">
+        <v>45950.507307974534</v>
+      </c>
+      <c r="F20" s="27">
+        <v>45950.507307974534</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I12" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="M12" s="30">
-        <v>0</v>
-      </c>
-      <c r="N12" s="30">
-        <v>0</v>
-      </c>
-      <c r="O12" s="30">
-        <v>0</v>
-      </c>
-      <c r="P12" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q12" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="30" t="s">
+      <c r="J20" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K20" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L20" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="M20" s="26">
+        <v>0</v>
+      </c>
+      <c r="N20" s="26">
+        <v>0</v>
+      </c>
+      <c r="O20" s="26">
+        <v>0</v>
+      </c>
+      <c r="P20" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q20" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="31">
-        <v>45943.454216377315</v>
-      </c>
-      <c r="F13" s="31">
-        <v>45950.519221319446</v>
-      </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="30" t="s">
+      <c r="D21" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="27">
+        <v>45950.506925208334</v>
+      </c>
+      <c r="F21" s="27">
+        <v>45950.506925208334</v>
+      </c>
+      <c r="G21" s="27"/>
+      <c r="H21" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I13" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="L13" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="M13" s="30">
-        <v>0</v>
-      </c>
-      <c r="N13" s="30">
-        <v>0</v>
-      </c>
-      <c r="O13" s="30">
-        <v>0</v>
-      </c>
-      <c r="P13" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q13" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" s="30" t="s">
+      <c r="J21" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="M21" s="26">
+        <v>0</v>
+      </c>
+      <c r="N21" s="26">
+        <v>0</v>
+      </c>
+      <c r="O21" s="26">
+        <v>0</v>
+      </c>
+      <c r="P21" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q21" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="31">
-        <v>45950.457830729167</v>
-      </c>
-      <c r="F14" s="31">
-        <v>45950.513444525466</v>
-      </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="30" t="s">
+      <c r="D22" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E22" s="27">
+        <v>45950.520432638892</v>
+      </c>
+      <c r="F22" s="27">
+        <v>45950.520432638892</v>
+      </c>
+      <c r="G22" s="27"/>
+      <c r="H22" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I14" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="L14" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="M14" s="30">
-        <v>0</v>
-      </c>
-      <c r="N14" s="30">
-        <v>0</v>
-      </c>
-      <c r="O14" s="30">
-        <v>0</v>
-      </c>
-      <c r="P14" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q14" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="30" t="s">
+      <c r="J22" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="M22" s="26">
+        <v>0</v>
+      </c>
+      <c r="N22" s="26">
+        <v>0</v>
+      </c>
+      <c r="O22" s="26">
+        <v>0</v>
+      </c>
+      <c r="P22" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q22" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" s="31">
-        <v>45950.45394861111</v>
-      </c>
-      <c r="F15" s="31">
-        <v>45950.513370104163</v>
-      </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30" t="s">
+      <c r="D23" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="27">
+        <v>45950.520298958334</v>
+      </c>
+      <c r="F23" s="27">
+        <v>45950.520298958334</v>
+      </c>
+      <c r="G23" s="27"/>
+      <c r="H23" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I15" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J15" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K15" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="L15" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="M15" s="30">
-        <v>0</v>
-      </c>
-      <c r="N15" s="30">
-        <v>0</v>
-      </c>
-      <c r="O15" s="30">
-        <v>0</v>
-      </c>
-      <c r="P15" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q15" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B16" s="30" t="s">
+      <c r="J23" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K23" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="M23" s="26">
+        <v>0</v>
+      </c>
+      <c r="N23" s="26">
+        <v>0</v>
+      </c>
+      <c r="O23" s="26">
+        <v>0</v>
+      </c>
+      <c r="P23" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q23" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="30" t="s">
+      <c r="D24" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24" s="27">
+        <v>45950.520159583335</v>
+      </c>
+      <c r="F24" s="27">
+        <v>45950.520159583335</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J24" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K24" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E16" s="31">
-        <v>45950.512167835652</v>
-      </c>
-      <c r="F16" s="31">
-        <v>45950.51362597222</v>
-      </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="30" t="s">
+      <c r="L24" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="M24" s="26">
+        <v>0</v>
+      </c>
+      <c r="N24" s="26">
+        <v>0</v>
+      </c>
+      <c r="O24" s="26">
+        <v>0</v>
+      </c>
+      <c r="P24" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q24" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="27">
+        <v>45950.519979537035</v>
+      </c>
+      <c r="F25" s="27">
+        <v>45950.519979537035</v>
+      </c>
+      <c r="G25" s="27"/>
+      <c r="H25" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I16" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K16" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L16" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="M16" s="30">
-        <v>0</v>
-      </c>
-      <c r="N16" s="30">
-        <v>0</v>
-      </c>
-      <c r="O16" s="30">
-        <v>0</v>
-      </c>
-      <c r="P16" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q16" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="30" t="s">
+      <c r="J25" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K25" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L25" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="M25" s="26">
+        <v>0</v>
+      </c>
+      <c r="N25" s="26">
+        <v>0</v>
+      </c>
+      <c r="O25" s="26">
+        <v>0</v>
+      </c>
+      <c r="P25" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q25" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17" s="31">
-        <v>45950.512106817128</v>
-      </c>
-      <c r="F17" s="31">
-        <v>45950.513540092594</v>
-      </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="30" t="s">
+      <c r="D26" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="27">
+        <v>45950.519731238426</v>
+      </c>
+      <c r="F26" s="27">
+        <v>45950.519731238426</v>
+      </c>
+      <c r="G26" s="27"/>
+      <c r="H26" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I17" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L17" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="M17" s="30">
-        <v>0</v>
-      </c>
-      <c r="N17" s="30">
-        <v>0</v>
-      </c>
-      <c r="O17" s="30">
-        <v>0</v>
-      </c>
-      <c r="P17" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q17" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" s="31">
-        <v>45950.506588495373</v>
-      </c>
-      <c r="F18" s="31">
-        <v>45950.506588495373</v>
-      </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K18" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L18" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="M18" s="30">
-        <v>0</v>
-      </c>
-      <c r="N18" s="30">
-        <v>0</v>
-      </c>
-      <c r="O18" s="30">
-        <v>0</v>
-      </c>
-      <c r="P18" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q18" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="E19" s="31">
-        <v>45950.506292314814</v>
-      </c>
-      <c r="F19" s="31">
-        <v>45950.506292314814</v>
-      </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K19" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L19" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="M19" s="30">
-        <v>0</v>
-      </c>
-      <c r="N19" s="30">
-        <v>0</v>
-      </c>
-      <c r="O19" s="30">
-        <v>0</v>
-      </c>
-      <c r="P19" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q19" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="31">
-        <v>45950.507307974534</v>
-      </c>
-      <c r="F20" s="31">
-        <v>45950.507307974534</v>
-      </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K20" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L20" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="M20" s="30">
-        <v>0</v>
-      </c>
-      <c r="N20" s="30">
-        <v>0</v>
-      </c>
-      <c r="O20" s="30">
-        <v>0</v>
-      </c>
-      <c r="P20" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q20" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" s="31">
-        <v>45950.506925208334</v>
-      </c>
-      <c r="F21" s="31">
-        <v>45950.506925208334</v>
-      </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K21" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L21" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="M21" s="30">
-        <v>0</v>
-      </c>
-      <c r="N21" s="30">
-        <v>0</v>
-      </c>
-      <c r="O21" s="30">
-        <v>0</v>
-      </c>
-      <c r="P21" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q21" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="30" t="s">
+      <c r="J26" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K26" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L26" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="31">
-        <v>45950.520432638892</v>
-      </c>
-      <c r="F22" s="31">
-        <v>45950.520432638892</v>
-      </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K22" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L22" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="M22" s="30">
-        <v>0</v>
-      </c>
-      <c r="N22" s="30">
-        <v>0</v>
-      </c>
-      <c r="O22" s="30">
-        <v>0</v>
-      </c>
-      <c r="P22" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q22" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="E23" s="31">
-        <v>45950.520298958334</v>
-      </c>
-      <c r="F23" s="31">
-        <v>45950.520298958334</v>
-      </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K23" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L23" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="M23" s="30">
-        <v>0</v>
-      </c>
-      <c r="N23" s="30">
-        <v>0</v>
-      </c>
-      <c r="O23" s="30">
-        <v>0</v>
-      </c>
-      <c r="P23" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q23" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="E24" s="31">
-        <v>45950.520159583335</v>
-      </c>
-      <c r="F24" s="31">
-        <v>45950.520159583335</v>
-      </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K24" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L24" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="M24" s="30">
-        <v>0</v>
-      </c>
-      <c r="N24" s="30">
-        <v>0</v>
-      </c>
-      <c r="O24" s="30">
-        <v>0</v>
-      </c>
-      <c r="P24" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q24" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="E25" s="31">
-        <v>45950.519979537035</v>
-      </c>
-      <c r="F25" s="31">
-        <v>45950.519979537035</v>
-      </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J25" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L25" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="M25" s="30">
-        <v>0</v>
-      </c>
-      <c r="N25" s="30">
-        <v>0</v>
-      </c>
-      <c r="O25" s="30">
-        <v>0</v>
-      </c>
-      <c r="P25" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q25" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="E26" s="31">
-        <v>45950.519731238426</v>
-      </c>
-      <c r="F26" s="31">
-        <v>45950.519731238426</v>
-      </c>
-      <c r="G26" s="31"/>
-      <c r="H26" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J26" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K26" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L26" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="M26" s="30">
-        <v>0</v>
-      </c>
-      <c r="N26" s="30">
-        <v>0</v>
-      </c>
-      <c r="O26" s="30">
-        <v>0</v>
-      </c>
-      <c r="P26" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q26" s="30">
+      <c r="M26" s="26">
+        <v>0</v>
+      </c>
+      <c r="N26" s="26">
+        <v>0</v>
+      </c>
+      <c r="O26" s="26">
+        <v>0</v>
+      </c>
+      <c r="P26" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q26" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="B30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" t="s">
         <v>161</v>
-      </c>
-      <c r="C30" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="29">
+        <v>96</v>
+      </c>
+      <c r="B31" s="25">
         <v>45936</v>
       </c>
-      <c r="C31" s="29">
+      <c r="C31" s="25">
         <v>45950</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="29">
+        <v>120</v>
+      </c>
+      <c r="B32" s="25">
         <v>45950</v>
       </c>
-      <c r="C32" s="29">
+      <c r="C32" s="25">
         <v>45961</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" s="29">
+        <v>130</v>
+      </c>
+      <c r="B33" s="25">
         <v>45961</v>
       </c>
-      <c r="C33" s="29">
+      <c r="C33" s="25">
         <v>45975</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B34" s="29">
+        <v>136</v>
+      </c>
+      <c r="B34" s="25">
         <v>45975</v>
       </c>
-      <c r="C34" s="29">
+      <c r="C34" s="25">
         <v>45990</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" s="29">
+        <v>141</v>
+      </c>
+      <c r="B35" s="25">
         <v>45990</v>
       </c>
-      <c r="C35" s="29">
+      <c r="C35" s="25">
         <v>46005</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B36" s="29">
+        <v>146</v>
+      </c>
+      <c r="B36" s="25">
         <v>46005</v>
       </c>
-      <c r="C36" s="29">
+      <c r="C36" s="25">
         <v>46021</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>152</v>
-      </c>
-      <c r="B37" s="29">
+        <v>151</v>
+      </c>
+      <c r="B37" s="25">
         <v>46021</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37" s="25">
         <v>46028</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q1" xr:uid="{5866E5C1-172E-4782-AFD1-E9BEE95982AD}"/>

</xml_diff>

<commit_message>
Update Cronograma.xlsx with latest changes
The Cronograma.xlsx file has been updated. Please review the latest schedule and ensure all timelines are up to date.
</commit_message>
<xml_diff>
--- a/Documentos Internos/Cronograma.xlsx
+++ b/Documentos Internos/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\GitHub\PDM_PA_50_10\Documentos Internos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B09AF3-809F-4592-8BB6-87F8088D459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1565335F-530E-49BB-8A66-AD463BCBCAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -956,14 +956,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="F8" zoomScale="190" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1276,37 +1276,37 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="30" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="30" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="30" t="s">
+      <c r="N1" s="29"/>
+      <c r="O1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="31"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="30">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
@@ -1342,7 +1342,7 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="60">
-      <c r="A3" s="29"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -1380,7 +1380,7 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" ht="44.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="82.5" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2">
@@ -1451,7 +1451,7 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="45">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="2">
         <v>7</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="29"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" ht="44.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="2">
         <v>9</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="45">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2">
@@ -1596,7 +1596,7 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="29"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="2">
         <v>11</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="29"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="2">
         <v>12</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" ht="45">
-      <c r="A12" s="29"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="2">
         <v>13</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" ht="60">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
@@ -1739,7 +1739,7 @@
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="29"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="2">
         <v>15</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" ht="45">
-      <c r="A15" s="29"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="2">
         <v>16</v>
       </c>
@@ -1809,7 +1809,7 @@
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="29"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="2">
         <v>17</v>
       </c>
@@ -1843,7 +1843,7 @@
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="29"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="2">
         <v>18</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2">
@@ -1915,7 +1915,7 @@
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" ht="30">
-      <c r="A19" s="29"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -1946,6 +1946,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
@@ -1953,11 +1958,6 @@
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{0A4A7E6F-5B19-4043-8AA1-14A479757A24}"/>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895AAF2E-62E0-4D99-9699-CE3C7B3F175D}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A7" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2343,17 +2343,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866E5C1-172E-4782-AFD1-E9BEE95982AD}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="136" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3007,7 +3008,9 @@
       <c r="F13" s="27">
         <v>45950.519221319446</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="27">
+        <v>45979</v>
+      </c>
       <c r="H13" s="26" t="s">
         <v>92</v>
       </c>
@@ -3109,7 +3112,9 @@
       <c r="F15" s="27">
         <v>45950.513370104163</v>
       </c>
-      <c r="G15" s="27"/>
+      <c r="G15" s="27">
+        <v>45970</v>
+      </c>
       <c r="H15" s="26" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Add authentication, validation, and refactor routes/controllers
Introduced authentication middleware using Firebase Admin, added Zod-based validation schemas for 'apoiados' and 'funcionarios', and refactored controllers and routes to use these schemas and new RESTful conventions. All API endpoints for 'apoiados' and 'funcionarios' are now protected and expect validated input. Updated Firebase config export, improved error handling, and replaced default route exports with named exports for better modularity.
</commit_message>
<xml_diff>
--- a/Documentos Internos/Cronograma.xlsx
+++ b/Documentos Internos/Cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\GitHub\PDM_PA_50_10\Documentos Internos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1565335F-530E-49BB-8A66-AD463BCBCAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC5408-666D-4366-BE20-44906109C2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -275,9 +275,6 @@
     <t>:: Casos de uso </t>
   </si>
   <si>
-    <t>:: Diagrama de modelo de dados (ER) </t>
-  </si>
-  <si>
     <t>::Diagrama de Estados</t>
   </si>
   <si>
@@ -518,9 +515,6 @@
     <t>PAP-3</t>
   </si>
   <si>
-    <t>Diagrama de modelo de dados (ER)</t>
-  </si>
-  <si>
     <t>PAP-13</t>
   </si>
   <si>
@@ -639,6 +633,12 @@
   </si>
   <si>
     <t>:: Diagrama de dominio</t>
+  </si>
+  <si>
+    <t>:: Diagrama de Classes</t>
+  </si>
+  <si>
+    <t>Diagrama de Classes</t>
   </si>
 </sst>
 </file>
@@ -956,14 +956,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1276,37 +1276,37 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="28" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="28" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="28" t="s">
+      <c r="J1" s="31"/>
+      <c r="K1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="28" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="29"/>
-      <c r="O1" s="28" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="29"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="30">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
@@ -1342,7 +1342,7 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="60">
-      <c r="A3" s="31"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>26</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O3" s="3">
         <v>27</v>
@@ -1380,7 +1380,7 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" ht="44.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="82.5" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2">
@@ -1451,7 +1451,7 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="45">
-      <c r="A6" s="31"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2">
         <v>7</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="3">
         <v>14</v>
@@ -1486,7 +1486,7 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="31"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" ht="44.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2">
         <v>9</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="45">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2">
@@ -1572,7 +1572,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" s="3">
         <v>4</v>
@@ -1596,7 +1596,7 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="31"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2">
         <v>11</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="31"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2">
         <v>12</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" ht="45">
-      <c r="A12" s="31"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2">
         <v>13</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="3">
         <v>25</v>
@@ -1700,7 +1700,7 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" ht="60">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
@@ -1731,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O13" s="3">
         <v>6</v>
@@ -1739,7 +1739,7 @@
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="31"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2">
         <v>15</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" ht="45">
-      <c r="A15" s="31"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2">
         <v>16</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="3">
         <v>16</v>
@@ -1809,7 +1809,7 @@
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="31"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2">
         <v>17</v>
       </c>
@@ -1843,7 +1843,7 @@
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="31"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2">
         <v>18</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="28" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2">
@@ -1915,7 +1915,7 @@
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" ht="30">
-      <c r="A19" s="31"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -1946,11 +1946,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
@@ -1958,6 +1953,11 @@
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{0A4A7E6F-5B19-4043-8AA1-14A479757A24}"/>
@@ -1975,7 +1975,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2124,19 +2124,19 @@
     </row>
     <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="20" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="B23" s="17"/>
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B24" s="17"/>
     </row>
     <row r="25" spans="1:5" ht="15.75">
       <c r="A25" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="17"/>
     </row>
@@ -2161,7 +2161,7 @@
     <row r="29" spans="1:5" ht="15.75">
       <c r="A29" s="17"/>
       <c r="B29" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75">
@@ -2170,25 +2170,25 @@
     </row>
     <row r="31" spans="1:5" ht="15.75">
       <c r="A31" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="22"/>
     </row>
     <row r="32" spans="1:5" ht="15.75">
       <c r="A32" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="22"/>
     </row>
     <row r="33" spans="1:2" ht="15.75">
       <c r="A33" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" s="17"/>
     </row>
     <row r="34" spans="1:2" ht="15.75">
       <c r="A34" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="17"/>
     </row>
@@ -2201,12 +2201,12 @@
     <row r="36" spans="1:2" ht="15.75">
       <c r="A36" s="17"/>
       <c r="B36" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75">
       <c r="A37" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="17"/>
     </row>
@@ -2216,13 +2216,13 @@
     </row>
     <row r="39" spans="1:2" ht="15.75">
       <c r="A39" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" s="22"/>
     </row>
     <row r="40" spans="1:2" ht="15.75">
       <c r="A40" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="22"/>
     </row>
@@ -2234,19 +2234,19 @@
     </row>
     <row r="42" spans="1:2" ht="15.75">
       <c r="A42" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="17"/>
     </row>
     <row r="43" spans="1:2" ht="15.75">
       <c r="A43" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="17"/>
     </row>
     <row r="44" spans="1:2" ht="15.75">
       <c r="A44" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="17"/>
     </row>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="47" spans="1:2" ht="15.75">
       <c r="A47" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="17"/>
     </row>
@@ -2272,19 +2272,19 @@
     </row>
     <row r="49" spans="1:2" ht="15.75">
       <c r="A49" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="17"/>
     </row>
     <row r="50" spans="1:2" ht="15.75">
       <c r="A50" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" s="17"/>
     </row>
     <row r="51" spans="1:2" ht="15.75">
       <c r="A51" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="17"/>
     </row>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="53" spans="1:2" ht="15.75">
       <c r="A53" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="17"/>
     </row>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="55" spans="1:2" ht="15.75">
       <c r="A55" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="17"/>
     </row>
     <row r="56" spans="1:2" ht="15.75">
       <c r="A56" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="17"/>
     </row>
@@ -2343,87 +2343,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866E5C1-172E-4782-AFD1-E9BEE95982AD}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="136" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="O1" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="P1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="Q1" s="26" t="s">
         <v>86</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="E2" s="27">
         <v>45950.510974328703</v>
@@ -2435,31 +2434,31 @@
         <v>45950.511442997682</v>
       </c>
       <c r="H2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="J2" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="L2" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="M2" s="26">
+        <v>0</v>
+      </c>
+      <c r="N2" s="26">
+        <v>0</v>
+      </c>
+      <c r="O2" s="26">
+        <v>0</v>
+      </c>
+      <c r="P2" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M2" s="26">
-        <v>0</v>
-      </c>
-      <c r="N2" s="26">
-        <v>0</v>
-      </c>
-      <c r="O2" s="26">
-        <v>0</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="Q2" s="26">
         <v>0</v>
@@ -2467,16 +2466,16 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>99</v>
       </c>
       <c r="E3" s="27">
         <v>45950.511326782405</v>
@@ -2488,31 +2487,31 @@
         <v>45950.511427962963</v>
       </c>
       <c r="H3" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="J3" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="K3" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="M3" s="26">
+        <v>0</v>
+      </c>
+      <c r="N3" s="26">
+        <v>0</v>
+      </c>
+      <c r="O3" s="26">
+        <v>0</v>
+      </c>
+      <c r="P3" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M3" s="26">
-        <v>0</v>
-      </c>
-      <c r="N3" s="26">
-        <v>0</v>
-      </c>
-      <c r="O3" s="26">
-        <v>0</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="Q3" s="26">
         <v>0</v>
@@ -2520,16 +2519,16 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>102</v>
       </c>
       <c r="E4" s="27">
         <v>45943.456266875</v>
@@ -2541,31 +2540,31 @@
         <v>45950.510832662039</v>
       </c>
       <c r="H4" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="J4" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="K4" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L4" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="M4" s="26">
+        <v>0</v>
+      </c>
+      <c r="N4" s="26">
+        <v>0</v>
+      </c>
+      <c r="O4" s="26">
+        <v>0</v>
+      </c>
+      <c r="P4" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M4" s="26">
-        <v>0</v>
-      </c>
-      <c r="N4" s="26">
-        <v>0</v>
-      </c>
-      <c r="O4" s="26">
-        <v>0</v>
-      </c>
-      <c r="P4" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="Q4" s="26">
         <v>0</v>
@@ -2573,16 +2572,16 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>105</v>
       </c>
       <c r="E5" s="27">
         <v>45943.430894224533</v>
@@ -2594,31 +2593,31 @@
         <v>45950.510795578703</v>
       </c>
       <c r="H5" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="K5" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L5" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="26">
+        <v>0</v>
+      </c>
+      <c r="N5" s="26">
+        <v>0</v>
+      </c>
+      <c r="O5" s="26">
+        <v>0</v>
+      </c>
+      <c r="P5" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M5" s="26">
-        <v>0</v>
-      </c>
-      <c r="N5" s="26">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26">
-        <v>0</v>
-      </c>
-      <c r="P5" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="Q5" s="26">
         <v>0</v>
@@ -2626,13 +2625,13 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>89</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>90</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>32</v>
@@ -2647,19 +2646,19 @@
         <v>45950.510773969909</v>
       </c>
       <c r="H6" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="J6" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="K6" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M6" s="26">
         <v>0</v>
@@ -2671,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q6" s="26">
         <v>0</v>
@@ -2679,16 +2678,16 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>108</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>109</v>
       </c>
       <c r="E7" s="27">
         <v>45943.430474560184</v>
@@ -2700,31 +2699,31 @@
         <v>45950.510754120369</v>
       </c>
       <c r="H7" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="J7" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="K7" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L7" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="M7" s="26">
+        <v>0</v>
+      </c>
+      <c r="N7" s="26">
+        <v>0</v>
+      </c>
+      <c r="O7" s="26">
+        <v>0</v>
+      </c>
+      <c r="P7" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M7" s="26">
-        <v>0</v>
-      </c>
-      <c r="N7" s="26">
-        <v>0</v>
-      </c>
-      <c r="O7" s="26">
-        <v>0</v>
-      </c>
-      <c r="P7" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="Q7" s="26">
         <v>0</v>
@@ -2732,16 +2731,16 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>111</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>112</v>
       </c>
       <c r="E8" s="27">
         <v>45940.606958912038</v>
@@ -2753,31 +2752,31 @@
         <v>45950.510734444448</v>
       </c>
       <c r="H8" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="J8" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="K8" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L8" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" s="26">
+        <v>0</v>
+      </c>
+      <c r="N8" s="26">
+        <v>0</v>
+      </c>
+      <c r="O8" s="26">
+        <v>0</v>
+      </c>
+      <c r="P8" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M8" s="26">
-        <v>0</v>
-      </c>
-      <c r="N8" s="26">
-        <v>0</v>
-      </c>
-      <c r="O8" s="26">
-        <v>0</v>
-      </c>
-      <c r="P8" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="Q8" s="26">
         <v>0</v>
@@ -2785,16 +2784,16 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>114</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>115</v>
       </c>
       <c r="E9" s="27">
         <v>45943.431502662039</v>
@@ -2806,31 +2805,31 @@
         <v>45950.510677256942</v>
       </c>
       <c r="H9" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="J9" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="26" t="s">
-        <v>94</v>
-      </c>
       <c r="K9" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L9" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="M9" s="26">
+        <v>0</v>
+      </c>
+      <c r="N9" s="26">
+        <v>0</v>
+      </c>
+      <c r="O9" s="26">
+        <v>0</v>
+      </c>
+      <c r="P9" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="M9" s="26">
-        <v>0</v>
-      </c>
-      <c r="N9" s="26">
-        <v>0</v>
-      </c>
-      <c r="O9" s="26">
-        <v>0</v>
-      </c>
-      <c r="P9" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="Q9" s="26">
         <v>0</v>
@@ -2838,16 +2837,16 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>117</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>118</v>
       </c>
       <c r="E10" s="27">
         <v>45943.45384840278</v>
@@ -2857,20 +2856,20 @@
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I10" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J10" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="L10" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="K10" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="M10" s="26">
         <v>0</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q10" s="26">
         <v>0</v>
@@ -2889,16 +2888,16 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D11" s="26" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="E11" s="27">
         <v>45940.607197754631</v>
@@ -2908,20 +2907,20 @@
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J11" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="M11" s="26">
         <v>0</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q11" s="26">
         <v>0</v>
@@ -2940,16 +2939,16 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D12" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E12" s="27">
         <v>45947.650316388892</v>
@@ -2959,20 +2958,20 @@
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J12" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="L12" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="K12" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="L12" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="M12" s="26">
         <v>0</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q12" s="26">
         <v>0</v>
@@ -2991,16 +2990,16 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D13" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E13" s="27">
         <v>45943.454216377315</v>
@@ -3012,20 +3011,20 @@
         <v>45979</v>
       </c>
       <c r="H13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J13" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="K13" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="L13" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="M13" s="26">
         <v>0</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q13" s="26">
         <v>0</v>
@@ -3044,16 +3043,16 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D14" s="26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E14" s="27">
         <v>45950.457830729167</v>
@@ -3063,19 +3062,19 @@
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J14" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M14" s="26">
         <v>0</v>
@@ -3087,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q14" s="26">
         <v>0</v>
@@ -3095,16 +3094,16 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B15" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D15" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E15" s="27">
         <v>45950.45394861111</v>
@@ -3116,19 +3115,19 @@
         <v>45970</v>
       </c>
       <c r="H15" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J15" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M15" s="26">
         <v>0</v>
@@ -3140,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q15" s="26">
         <v>0</v>
@@ -3148,16 +3147,16 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D16" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E16" s="27">
         <v>45950.512167835652</v>
@@ -3167,19 +3166,19 @@
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I16" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J16" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M16" s="26">
         <v>0</v>
@@ -3191,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q16" s="26">
         <v>0</v>
@@ -3199,16 +3198,16 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B17" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D17" s="26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E17" s="27">
         <v>45950.512106817128</v>
@@ -3218,19 +3217,19 @@
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I17" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J17" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M17" s="26">
         <v>0</v>
@@ -3242,7 +3241,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q17" s="26">
         <v>0</v>
@@ -3250,16 +3249,16 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B18" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D18" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E18" s="27">
         <v>45950.506588495373</v>
@@ -3269,19 +3268,19 @@
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J18" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M18" s="26">
         <v>0</v>
@@ -3293,7 +3292,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q18" s="26">
         <v>0</v>
@@ -3301,16 +3300,16 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B19" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D19" s="26" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E19" s="27">
         <v>45950.506292314814</v>
@@ -3320,19 +3319,19 @@
       </c>
       <c r="G19" s="27"/>
       <c r="H19" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J19" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M19" s="26">
         <v>0</v>
@@ -3344,7 +3343,7 @@
         <v>0</v>
       </c>
       <c r="P19" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q19" s="26">
         <v>0</v>
@@ -3352,16 +3351,16 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B20" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D20" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E20" s="27">
         <v>45950.507307974534</v>
@@ -3371,19 +3370,19 @@
       </c>
       <c r="G20" s="27"/>
       <c r="H20" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I20" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J20" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M20" s="26">
         <v>0</v>
@@ -3395,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q20" s="26">
         <v>0</v>
@@ -3403,16 +3402,16 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B21" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D21" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E21" s="27">
         <v>45950.506925208334</v>
@@ -3422,19 +3421,19 @@
       </c>
       <c r="G21" s="27"/>
       <c r="H21" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J21" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M21" s="26">
         <v>0</v>
@@ -3446,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q21" s="26">
         <v>0</v>
@@ -3454,16 +3453,16 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B22" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D22" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E22" s="27">
         <v>45950.520432638892</v>
@@ -3473,19 +3472,19 @@
       </c>
       <c r="G22" s="27"/>
       <c r="H22" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J22" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K22" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M22" s="26">
         <v>0</v>
@@ -3497,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="P22" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q22" s="26">
         <v>0</v>
@@ -3505,16 +3504,16 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D23" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E23" s="27">
         <v>45950.520298958334</v>
@@ -3524,19 +3523,19 @@
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I23" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J23" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K23" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L23" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M23" s="26">
         <v>0</v>
@@ -3548,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q23" s="26">
         <v>0</v>
@@ -3556,16 +3555,16 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B24" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D24" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E24" s="27">
         <v>45950.520159583335</v>
@@ -3575,19 +3574,19 @@
       </c>
       <c r="G24" s="27"/>
       <c r="H24" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I24" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J24" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K24" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L24" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M24" s="26">
         <v>0</v>
@@ -3599,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q24" s="26">
         <v>0</v>
@@ -3607,16 +3606,16 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B25" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D25" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E25" s="27">
         <v>45950.519979537035</v>
@@ -3626,19 +3625,19 @@
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J25" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K25" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L25" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M25" s="26">
         <v>0</v>
@@ -3650,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q25" s="26">
         <v>0</v>
@@ -3658,16 +3657,16 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B26" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="D26" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E26" s="27">
         <v>45950.519731238426</v>
@@ -3677,19 +3676,19 @@
       </c>
       <c r="G26" s="27"/>
       <c r="H26" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I26" s="26" t="s">
-        <v>93</v>
-      </c>
       <c r="J26" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K26" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L26" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M26" s="26">
         <v>0</v>
@@ -3701,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q26" s="26">
         <v>0</v>
@@ -3709,15 +3708,15 @@
     </row>
     <row r="30" spans="1:17">
       <c r="B30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" s="25">
         <v>45936</v>
@@ -3728,7 +3727,7 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B32" s="25">
         <v>45950</v>
@@ -3743,7 +3742,7 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B33" s="25">
         <v>45961</v>
@@ -3758,7 +3757,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B34" s="25">
         <v>45975</v>
@@ -3773,7 +3772,7 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B35" s="25">
         <v>45990</v>
@@ -3788,7 +3787,7 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B36" s="25">
         <v>46005</v>
@@ -3803,7 +3802,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B37" s="25">
         <v>46021</v>

</xml_diff>

<commit_message>
Remove backend Firebase functions and configs
Deleted all files related to the Backend Firebase implementation, including configuration, Firestore rules, indexes, and all Cloud Functions source code. Added new domain diagram files. Updated internal schedule document.
</commit_message>
<xml_diff>
--- a/Documentos Internos/Cronograma.xlsx
+++ b/Documentos Internos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\GitHub\PDM_PA_50_10\Documentos Internos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC5408-666D-4366-BE20-44906109C2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132B5F15-6874-4DDA-81B4-1E755243FFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="164">
   <si>
     <t>MÊS</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>Diagrama de Classes</t>
+  </si>
+  <si>
+    <t>Nandes e Tierri</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView topLeftCell="F8" zoomScale="190" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C6" zoomScale="104" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -1974,7 +1977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895AAF2E-62E0-4D99-9699-CE3C7B3F175D}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -2344,7 +2347,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2905,7 +2908,9 @@
       <c r="F11" s="27">
         <v>45950.519361666666</v>
       </c>
-      <c r="G11" s="27"/>
+      <c r="G11" s="27">
+        <v>45985</v>
+      </c>
       <c r="H11" s="26" t="s">
         <v>91</v>
       </c>
@@ -2916,7 +2921,7 @@
         <v>118</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="L11" s="26" t="s">
         <v>119</v>
@@ -2967,7 +2972,7 @@
         <v>118</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="L12" s="26" t="s">
         <v>119</v>
@@ -3020,7 +3025,7 @@
         <v>118</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="L13" s="26" t="s">
         <v>119</v>
@@ -3226,7 +3231,7 @@
         <v>118</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="L17" s="26" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
Add admin role and collaborators management features
Introduces the 'Admin' user role and updates user role logic throughout the app. Adds UI and ViewModel for listing, promoting, demoting, and deleting collaborators, with admin-only access to these features. Updates profile creation to allow role selection, restricts account deletion for admins, and adjusts menu options based on user role. Also includes minor UI and navigation improvements.
</commit_message>
<xml_diff>
--- a/Documentos Internos/Cronograma.xlsx
+++ b/Documentos Internos/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\GitHub\PDM_PA_50_10\Documentos Internos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F909D5A-7070-451E-8369-4ED548418937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CDF630-006F-4F44-8225-B2D9FA6121C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -959,14 +959,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1279,37 +1279,37 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="28" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="28" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="28" t="s">
+      <c r="J1" s="31"/>
+      <c r="K1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="28" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="29"/>
-      <c r="O1" s="28" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="29"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="30">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2">
@@ -1345,7 +1345,7 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="60">
-      <c r="A3" s="31"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -1383,7 +1383,7 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" ht="44.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -1419,7 +1419,7 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" ht="82.5" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2">
@@ -1454,7 +1454,7 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="45">
-      <c r="A6" s="31"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2">
         <v>7</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="31"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" ht="44.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2">
         <v>9</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="45">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2">
@@ -1599,7 +1599,7 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="31"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2">
         <v>11</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="31"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2">
         <v>12</v>
       </c>
@@ -1665,7 +1665,7 @@
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" ht="45">
-      <c r="A12" s="31"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2">
         <v>13</v>
       </c>
@@ -1703,7 +1703,7 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" ht="60">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
@@ -1742,7 +1742,7 @@
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="31"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2">
         <v>15</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" ht="45">
-      <c r="A15" s="31"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2">
         <v>16</v>
       </c>
@@ -1812,7 +1812,7 @@
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="31"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2">
         <v>17</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="31"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2">
         <v>18</v>
       </c>
@@ -1880,7 +1880,7 @@
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="28" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2">
@@ -1918,7 +1918,7 @@
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" ht="30">
-      <c r="A19" s="31"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -1949,11 +1949,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
@@ -1961,6 +1956,11 @@
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{0A4A7E6F-5B19-4043-8AA1-14A479757A24}"/>
@@ -1977,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895AAF2E-62E0-4D99-9699-CE3C7B3F175D}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A37" activeCellId="2" sqref="A33:A35 B36 A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2184,31 +2184,31 @@
       <c r="B32" s="22"/>
     </row>
     <row r="33" spans="1:2" ht="15.75">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="17"/>
     </row>
     <row r="34" spans="1:2" ht="15.75">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B34" s="17"/>
     </row>
     <row r="35" spans="1:2" ht="15.75">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="17"/>
     </row>
     <row r="36" spans="1:2" ht="15.75">
       <c r="A36" s="17"/>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="24" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="24" t="s">
         <v>52</v>
       </c>
       <c r="B37" s="17"/>

</xml_diff>